<commit_message>
add base command for bot
</commit_message>
<xml_diff>
--- a/app/table.xlsx
+++ b/app/table.xlsx
@@ -11,12 +11,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>ID</t>
   </si>
   <si>
     <t>Value</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
 </sst>
 </file>
@@ -393,7 +411,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B8"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -404,8 +422,64 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add eslint and prettier
</commit_message>
<xml_diff>
--- a/app/table.xlsx
+++ b/app/table.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>ID</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t>0</t>
+  </si>
+  <si>
+    <t>12</t>
   </si>
 </sst>
 </file>
@@ -411,7 +414,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B10"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -478,6 +481,22 @@
         <v>100</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>